<commit_message>
Tidy up headers & label columns for GeoFabric
</commit_message>
<xml_diff>
--- a/crosswalks/Geofabric-IUCNGET/Geofabric-IUCNGET.xlsx
+++ b/crosswalks/Geofabric-IUCNGET/Geofabric-IUCNGET.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ecosystem-typology\crosswalks\Geofabric-IUCNGET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BEDB47-EB1A-4770-975B-17873C9987E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C430913-18EF-4039-BE42-7989259A5A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9060" yWindow="2460" windowWidth="19425" windowHeight="15345" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
+    <workbookView xWindow="690" yWindow="8295" windowWidth="29115" windowHeight="10815" activeTab="1" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
   <sheets>
     <sheet name="header" sheetId="5" r:id="rId1"/>
@@ -737,7 +737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74DD23B2-5C24-4E92-A3A3-39F13C78738A}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9:XFD19"/>
     </sheetView>
   </sheetViews>
@@ -795,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACFEC63-F603-4D93-B073-540A32B07BA6}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3:N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,8 +899,8 @@
         <v>70</v>
       </c>
       <c r="N2" s="7" t="str">
-        <f>_xlfn.CONCAT(B2, " - mapping to IUCN GET")</f>
-        <v>Swamps - perennial - mapping to IUCN GET</v>
+        <f>_xlfn.CONCAT(B2, " - mapping to IUCN GET - ", ROW(B2)-1 )</f>
+        <v>Swamps - perennial - mapping to IUCN GET - 1</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -941,8 +941,8 @@
         <v>70</v>
       </c>
       <c r="N3" s="7" t="str">
-        <f t="shared" ref="N3:N22" si="0">_xlfn.CONCAT(B3, " - mapping to IUCN GET")</f>
-        <v>Swamps - perennial - mapping to IUCN GET</v>
+        <f t="shared" ref="N3:N22" si="0">_xlfn.CONCAT(B3, " - mapping to IUCN GET - ", ROW(B3)-1 )</f>
+        <v>Swamps - perennial - mapping to IUCN GET - 2</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -981,7 +981,7 @@
       </c>
       <c r="N4" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>Swamps - nonperennial - mapping to IUCN GET</v>
+        <v>Swamps - nonperennial - mapping to IUCN GET - 3</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="N5" s="7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> - mapping to IUCN GET</v>
+        <v xml:space="preserve"> - mapping to IUCN GET - 4</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1050,7 +1050,7 @@
       </c>
       <c r="N6" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>Swamps - nonperennial - mapping to IUCN GET</v>
+        <v>Swamps - nonperennial - mapping to IUCN GET - 5</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1092,7 +1092,7 @@
       </c>
       <c r="N7" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>Rivers (minor) - perennial - mapping to IUCN GET</v>
+        <v>Rivers (minor) - perennial - mapping to IUCN GET - 6</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1134,7 +1134,7 @@
       </c>
       <c r="N8" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>Rivers (major) - perennial - mapping to IUCN GET</v>
+        <v>Rivers (major) - perennial - mapping to IUCN GET - 7</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1173,7 +1173,7 @@
       </c>
       <c r="N9" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>Rivers (minor) - nonperennial - mapping to IUCN GET</v>
+        <v>Rivers (minor) - nonperennial - mapping to IUCN GET - 8</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1215,7 +1215,7 @@
       </c>
       <c r="N10" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>Rivers (minor) - nonperennial - mapping to IUCN GET</v>
+        <v>Rivers (minor) - nonperennial - mapping to IUCN GET - 9</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="N11" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>Rivers (major) - nonperennial - mapping to IUCN GET</v>
+        <v>Rivers (major) - nonperennial - mapping to IUCN GET - 10</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1296,7 +1296,7 @@
       </c>
       <c r="N12" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>Rivers (major) - nonperennial - mapping to IUCN GET</v>
+        <v>Rivers (major) - nonperennial - mapping to IUCN GET - 11</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="N13" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>Lakes - perennial - mapping to IUCN GET</v>
+        <v>Lakes - perennial - mapping to IUCN GET - 12</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1380,7 +1380,7 @@
       </c>
       <c r="N14" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>Lakes - perennial - mapping to IUCN GET</v>
+        <v>Lakes - perennial - mapping to IUCN GET - 13</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1419,7 +1419,7 @@
       </c>
       <c r="N15" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>Lakes - nonperennial - mapping to IUCN GET</v>
+        <v>Lakes - nonperennial - mapping to IUCN GET - 14</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1458,7 +1458,7 @@
       </c>
       <c r="N16" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>Lakes - nonperennial - mapping to IUCN GET</v>
+        <v>Lakes - nonperennial - mapping to IUCN GET - 15</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -1500,7 +1500,7 @@
       </c>
       <c r="N17" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>Lakes - perennial - mapping to IUCN GET</v>
+        <v>Lakes - perennial - mapping to IUCN GET - 16</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -1542,7 +1542,7 @@
       </c>
       <c r="N18" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>Lakes - nonperennial - mapping to IUCN GET</v>
+        <v>Lakes - nonperennial - mapping to IUCN GET - 17</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -1584,7 +1584,7 @@
       </c>
       <c r="N19" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>Reservoirs - perennial - mapping to IUCN GET</v>
+        <v>Reservoirs - perennial - mapping to IUCN GET - 18</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -1626,7 +1626,7 @@
       </c>
       <c r="N20" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>Reservoirs - nonperennial - mapping to IUCN GET</v>
+        <v>Reservoirs - nonperennial - mapping to IUCN GET - 19</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -1656,7 +1656,7 @@
       </c>
       <c r="N21" s="7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> - mapping to IUCN GET</v>
+        <v xml:space="preserve"> - mapping to IUCN GET - 20</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1686,7 +1686,7 @@
       </c>
       <c r="N22" s="7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> - mapping to IUCN GET</v>
+        <v xml:space="preserve"> - mapping to IUCN GET - 21</v>
       </c>
     </row>
   </sheetData>
@@ -1696,82 +1696,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
-    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
-    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
-      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
-      <Description>63P7TJYCZHM3-28990658-16955</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100772FA3DF59B7CE49A6C16870444FDBEA" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1badbe4fae1da33fa4f3d33d98841982">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e444dda-df07-4069-8b25-4dfb1c3da75a" xmlns:ns3="72d9be16-af35-44ba-8991-a3db737bf75a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b20e6642ad5eb13a26fdf3049cd990" ns2:_="" ns3:_="">
     <xsd:import namespace="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
@@ -2047,34 +1971,83 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
-    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
+    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
+    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
+      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
+      <Description>63P7TJYCZHM3-28990658-16955</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66326C79-A0D3-4EA9-86BB-19E204621547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2091,4 +2064,31 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
+    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix subject URI - Geofabric
</commit_message>
<xml_diff>
--- a/crosswalks/Geofabric-IUCNGET/Geofabric-IUCNGET.xlsx
+++ b/crosswalks/Geofabric-IUCNGET/Geofabric-IUCNGET.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ecosystem-typology\crosswalks\Geofabric-IUCNGET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fcabc4d7e599448e/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C430913-18EF-4039-BE42-7989259A5A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEFD76D2-D440-48B4-AF28-5BBD483E6C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="8295" windowWidth="29115" windowHeight="10815" activeTab="1" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="34230" windowHeight="15435" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
   <sheets>
     <sheet name="header" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="89">
   <si>
     <t>semapv:ManualMappingCuration</t>
   </si>
@@ -54,61 +54,31 @@
     <t>Craig Macfarlane</t>
   </si>
   <si>
-    <t>geofabric:Lakes - perennial</t>
-  </si>
-  <si>
     <t>Lakes - perennial</t>
   </si>
   <si>
-    <t>geofabric:Lakes - nonperennial</t>
-  </si>
-  <si>
     <t>Lakes - nonperennial</t>
   </si>
   <si>
-    <t>geofabric:Swamps - perennial</t>
-  </si>
-  <si>
     <t>Swamps - perennial</t>
   </si>
   <si>
-    <t>geofabric:Swamps - nonperennial</t>
-  </si>
-  <si>
     <t>Swamps - nonperennial</t>
   </si>
   <si>
-    <t>geofabric:Reservoirs - perennial</t>
-  </si>
-  <si>
     <t>Reservoirs - perennial</t>
   </si>
   <si>
-    <t>geofabric:Reservoirs - nonperennial</t>
-  </si>
-  <si>
     <t>Reservoirs - nonperennial</t>
   </si>
   <si>
-    <t>geofabric:Rivers (major) - perennial</t>
-  </si>
-  <si>
     <t>Rivers (major) - perennial</t>
   </si>
   <si>
-    <t>geofabric:Rivers (major) - nonperennial</t>
-  </si>
-  <si>
     <t>Rivers (major) - nonperennial</t>
   </si>
   <si>
-    <t>geofabric:Rivers (minor) - perennial</t>
-  </si>
-  <si>
     <t>Rivers (minor) - perennial</t>
-  </si>
-  <si>
-    <t>geofabric:Rivers (minor) - nonperennial</t>
   </si>
   <si>
     <t>Rivers (minor) - nonperennial</t>
@@ -737,7 +707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74DD23B2-5C24-4E92-A3A3-39F13C78738A}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:XFD19"/>
     </sheetView>
   </sheetViews>
@@ -748,42 +718,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -795,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACFEC63-F603-4D93-B073-540A32B07BA6}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:N22"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,69 +783,70 @@
     <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="68.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="48.140625" customWidth="1"/>
     <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="L1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
+      <c r="A2" t="str">
+        <f t="shared" ref="A2:A4" si="0">_xlfn.CONCAT("geofabric:",   SUBSTITUTE( SUBSTITUTE( SUBSTITUTE(B2," ",""), "(", "-" ), ")", "-" )      )</f>
+        <v>geofabric:Swamps-perennial</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -890,13 +861,13 @@
         <v>45372</v>
       </c>
       <c r="J2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="K2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="M2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="N2" s="7" t="str">
         <f>_xlfn.CONCAT(B2, " - mapping to IUCN GET - ", ROW(B2)-1 )</f>
@@ -904,20 +875,21 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
+      <c r="A3" t="str">
+        <f t="shared" si="0"/>
+        <v>geofabric:Swamps-perennial</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="F3" t="s">
         <v>0</v>
@@ -932,34 +904,35 @@
         <v>45372</v>
       </c>
       <c r="J3" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="K3" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="M3" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="N3" s="7" t="str">
-        <f t="shared" ref="N3:N22" si="0">_xlfn.CONCAT(B3, " - mapping to IUCN GET - ", ROW(B3)-1 )</f>
+        <f t="shared" ref="N3:N22" si="1">_xlfn.CONCAT(B3, " - mapping to IUCN GET - ", ROW(B3)-1 )</f>
         <v>Swamps - perennial - mapping to IUCN GET - 2</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>geofabric:Swamps-nonperennial</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
@@ -974,22 +947,22 @@
         <v>45372</v>
       </c>
       <c r="J4" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="K4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="N4" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Swamps - nonperennial - mapping to IUCN GET - 3</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
         <v>0</v>
@@ -1004,31 +977,32 @@
         <v>45372</v>
       </c>
       <c r="K5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="M5" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="N5" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> - mapping to IUCN GET - 4</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
+      <c r="A6" t="str">
+        <f>_xlfn.CONCAT("geofabric:",   SUBSTITUTE( SUBSTITUTE( SUBSTITUTE(B6," ",""), "(", "-" ), ")", "-" )      )</f>
+        <v>geofabric:Swamps-nonperennial</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="F6" t="s">
         <v>0</v>
@@ -1043,31 +1017,32 @@
         <v>45372</v>
       </c>
       <c r="K6" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="M6" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="N6" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Swamps - nonperennial - mapping to IUCN GET - 5</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>21</v>
+      <c r="A7" t="str">
+        <f>_xlfn.CONCAT("geofabric:",   SUBSTITUTE( SUBSTITUTE( SUBSTITUTE(B7," ",""), "(", "-" ), ")", "-" )      )</f>
+        <v>geofabric:Rivers-minor--perennial</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F7" t="s">
         <v>0</v>
@@ -1082,34 +1057,35 @@
         <v>45372</v>
       </c>
       <c r="J7" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" t="s">
+        <v>62</v>
+      </c>
+      <c r="N7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>Rivers (minor) - perennial - mapping to IUCN GET - 6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f t="shared" ref="A8:A20" si="2">_xlfn.CONCAT("geofabric:",   SUBSTITUTE( SUBSTITUTE( SUBSTITUTE(B8," ",""), "(", "-" ), ")", "-" )      )</f>
+        <v>geofabric:Rivers-major--perennial</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
         <v>64</v>
       </c>
-      <c r="K7" t="s">
-        <v>63</v>
-      </c>
-      <c r="M7" t="s">
-        <v>72</v>
-      </c>
-      <c r="N7" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>Rivers (minor) - perennial - mapping to IUCN GET - 6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>74</v>
-      </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s">
         <v>0</v>
@@ -1124,34 +1100,35 @@
         <v>45372</v>
       </c>
       <c r="J8" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="K8" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="M8" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="N8" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Rivers (major) - perennial - mapping to IUCN GET - 7</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>23</v>
+      <c r="A9" t="str">
+        <f t="shared" si="2"/>
+        <v>geofabric:Rivers-minor--nonperennial</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="F9" t="s">
         <v>0</v>
@@ -1166,31 +1143,32 @@
         <v>45372</v>
       </c>
       <c r="J9" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="K9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="N9" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Rivers (minor) - nonperennial - mapping to IUCN GET - 8</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>23</v>
+      <c r="A10" t="str">
+        <f t="shared" si="2"/>
+        <v>geofabric:Rivers-minor--nonperennial</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
         <v>0</v>
@@ -1205,34 +1183,35 @@
         <v>45372</v>
       </c>
       <c r="J10" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="K10" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="M10" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="N10" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Rivers (minor) - nonperennial - mapping to IUCN GET - 9</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>19</v>
+      <c r="A11" t="str">
+        <f t="shared" si="2"/>
+        <v>geofabric:Rivers-major--nonperennial</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="F11" t="s">
         <v>0</v>
@@ -1247,34 +1226,35 @@
         <v>45372</v>
       </c>
       <c r="J11" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="K11" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="M11" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="N11" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Rivers (major) - nonperennial - mapping to IUCN GET - 10</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>19</v>
+      <c r="A12" t="str">
+        <f t="shared" si="2"/>
+        <v>geofabric:Rivers-major--nonperennial</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
         <v>0</v>
@@ -1289,31 +1269,32 @@
         <v>45372</v>
       </c>
       <c r="J12" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="K12" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="N12" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Rivers (major) - nonperennial - mapping to IUCN GET - 11</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" t="str">
+        <f t="shared" si="2"/>
+        <v>geofabric:Lakes-perennial</v>
+      </c>
+      <c r="B13" t="s">
         <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F13" t="s">
         <v>0</v>
@@ -1328,34 +1309,35 @@
         <v>45372</v>
       </c>
       <c r="J13" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="K13" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="M13" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="N13" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Lakes - perennial - mapping to IUCN GET - 12</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" t="str">
+        <f t="shared" si="2"/>
+        <v>geofabric:Lakes-perennial</v>
+      </c>
+      <c r="B14" t="s">
         <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F14" t="s">
         <v>0</v>
@@ -1370,34 +1352,35 @@
         <v>45372</v>
       </c>
       <c r="J14" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="K14" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="M14" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="N14" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Lakes - perennial - mapping to IUCN GET - 13</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>7</v>
+      <c r="A15" t="str">
+        <f t="shared" si="2"/>
+        <v>geofabric:Lakes-nonperennial</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F15" t="s">
         <v>0</v>
@@ -1412,31 +1395,32 @@
         <v>45372</v>
       </c>
       <c r="J15" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="K15" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="N15" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Lakes - nonperennial - mapping to IUCN GET - 14</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>7</v>
+      <c r="A16" t="str">
+        <f t="shared" si="2"/>
+        <v>geofabric:Lakes-nonperennial</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="F16" t="s">
         <v>0</v>
@@ -1451,31 +1435,32 @@
         <v>45372</v>
       </c>
       <c r="J16" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="K16" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="N16" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Lakes - nonperennial - mapping to IUCN GET - 15</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" t="str">
+        <f t="shared" si="2"/>
+        <v>geofabric:Lakes-perennial</v>
+      </c>
+      <c r="B17" t="s">
         <v>5</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="F17" t="s">
         <v>0</v>
@@ -1490,34 +1475,35 @@
         <v>45372</v>
       </c>
       <c r="J17" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="K17" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="M17" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="N17" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Lakes - perennial - mapping to IUCN GET - 16</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>7</v>
+      <c r="A18" t="str">
+        <f t="shared" si="2"/>
+        <v>geofabric:Lakes-nonperennial</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F18" t="s">
         <v>0</v>
@@ -1532,34 +1518,35 @@
         <v>45372</v>
       </c>
       <c r="J18" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="K18" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="M18" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="N18" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Lakes - nonperennial - mapping to IUCN GET - 17</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>13</v>
+      <c r="A19" t="str">
+        <f t="shared" si="2"/>
+        <v>geofabric:Reservoirs-perennial</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E19" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="F19" t="s">
         <v>0</v>
@@ -1574,34 +1561,35 @@
         <v>45372</v>
       </c>
       <c r="J19" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="K19" t="s">
+        <v>53</v>
+      </c>
+      <c r="M19" t="s">
         <v>63</v>
       </c>
-      <c r="M19" t="s">
-        <v>73</v>
-      </c>
       <c r="N19" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Reservoirs - perennial - mapping to IUCN GET - 18</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>15</v>
+      <c r="A20" t="str">
+        <f t="shared" si="2"/>
+        <v>geofabric:Reservoirs-nonperennial</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="F20" t="s">
         <v>0</v>
@@ -1616,25 +1604,25 @@
         <v>45372</v>
       </c>
       <c r="J20" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="K20" t="s">
+        <v>53</v>
+      </c>
+      <c r="M20" t="s">
         <v>63</v>
       </c>
-      <c r="M20" t="s">
-        <v>73</v>
-      </c>
       <c r="N20" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Reservoirs - nonperennial - mapping to IUCN GET - 19</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E21" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="F21" t="s">
         <v>0</v>
@@ -1649,22 +1637,22 @@
         <v>45372</v>
       </c>
       <c r="K21" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="M21" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="N21" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> - mapping to IUCN GET - 20</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E22" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="F22" t="s">
         <v>0</v>
@@ -1679,13 +1667,13 @@
         <v>45372</v>
       </c>
       <c r="K22" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="M22" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="N22" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> - mapping to IUCN GET - 21</v>
       </c>
     </row>
@@ -1696,6 +1684,65 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100772FA3DF59B7CE49A6C16870444FDBEA" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1badbe4fae1da33fa4f3d33d98841982">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e444dda-df07-4069-8b25-4dfb1c3da75a" xmlns:ns3="72d9be16-af35-44ba-8991-a3db737bf75a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b20e6642ad5eb13a26fdf3049cd990" ns2:_="" ns3:_="">
     <xsd:import namespace="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
@@ -1971,65 +2018,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2048,6 +2036,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66326C79-A0D3-4EA9-86BB-19E204621547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2066,22 +2070,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
   <ds:schemaRefs>

</xml_diff>